<commit_message>
Fixed experiment name in example data.
</commit_message>
<xml_diff>
--- a/example_data/example_data_lucas.xlsx
+++ b/example_data/example_data_lucas.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MSSA Biofilm Eradication CV" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="MSSA Biofilm Eradication TTC" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="MSSA Biofilm Inhibition CV" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="MSSA Biofilm Planktonic Inhibit" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="MSSA Planktonic Inhibition" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -131,7 +131,7 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1163,7 +1163,7 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>